<commit_message>
Added process and timeIndex as arguments to applyStateSpaceTransform
</commit_message>
<xml_diff>
--- a/docs/refactoring-4.1.x-to-5.0.0/Refactorings 4.1.x to 5.0.0.xlsx
+++ b/docs/refactoring-4.1.x-to-5.0.0/Refactorings 4.1.x to 5.0.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fries/Documents/Development/Repositories/finmath lib/docs/refactoring-4.1.x-to-5.0.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24AFC5A-4262-3946-BD65-66B69BAED7B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37AC1BE-510D-B142-8E43-2FE89DF75A81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="1500" windowWidth="28240" windowHeight="17560" xr2:uid="{C7647045-A3B7-E245-B7C6-0F67C8683C3E}"/>
+    <workbookView xWindow="2680" yWindow="1500" windowWidth="28240" windowHeight="17560" activeTab="2" xr2:uid="{C7647045-A3B7-E245-B7C6-0F67C8683C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>finmath-lib refactoring 4.x to 5.x</t>
   </si>
@@ -168,6 +168,27 @@
   </si>
   <si>
     <t>The default JDK of the library is Java 11. There is profile for Java 8 (-Pjava8)</t>
+  </si>
+  <si>
+    <t>applyStateSpaceTransform(MonteCarloProcess process, int timeIndex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	RandomVariable applyStateSpaceTransform(MonteCarloProcess process, int timeIndex, int componentIndex, RandomVariable randomVariable);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	default RandomVariable applyStateSpaceTransformInverse(MonteCarloProcess process, int timeIndex, final int componentIndex, final RandomVariable randomVariable) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	RandomVariable[] getInitialState(MonteCarloProcess process);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	RandomVariable getNumeraire(MonteCarloProcess process, double time) throws CalculationException;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	RandomVariable[] getDrift(MonteCarloProcess process, int timeIndex, RandomVariable[] realizationAtTimeIndex, RandomVariable[] realizationPredictor);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	RandomVariable[] getFactorLoading(MonteCarloProcess process, int timeIndex, int componentIndex, RandomVariable[] realizationAtTimeIndex);</t>
   </si>
 </sst>
 </file>
@@ -595,7 +616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA599C8B-EB72-AF45-A360-A73F96FC6FB1}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -860,10 +881,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A833A924-41AF-4F4B-B135-14135420801F}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -981,10 +1002,44 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added refactorings for 5.1 to docs.
</commit_message>
<xml_diff>
--- a/docs/refactoring-4.1.x-to-5.0.0/Refactorings 4.1.x to 5.0.0.xlsx
+++ b/docs/refactoring-4.1.x-to-5.0.0/Refactorings 4.1.x to 5.0.0.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fries/Documents/Development/Repositories/finmath lib/docs/refactoring-4.1.x-to-5.0.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABA6CF2-B5C5-3842-9958-C3FCABEE3EF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05D134E-3A30-AA42-9E30-87508F07FD62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5080" yWindow="1700" windowWidth="28240" windowHeight="17560" xr2:uid="{C7647045-A3B7-E245-B7C6-0F67C8683C3E}"/>
+    <workbookView xWindow="3840" yWindow="17540" windowWidth="31400" windowHeight="17560" xr2:uid="{C7647045-A3B7-E245-B7C6-0F67C8683C3E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Refactorings 4.1 to 5.0 Classes" sheetId="3" r:id="rId2"/>
     <sheet name="Refactorings 4.1 to 5.0 Methods" sheetId="5" r:id="rId3"/>
     <sheet name="Refactorings 4.0 to 4.1" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,14 +37,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
-  <si>
-    <t>finmath-lib refactoring 4.x to 5.x</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="67">
   <si>
     <t>Java 11</t>
   </si>
   <si>
+    <t>size of randomVariables int to long</t>
+  </si>
+  <si>
     <t>BrownianMotionLazyInit</t>
   </si>
   <si>
@@ -204,26 +207,44 @@
     <t>Refactorings of Interfaces and Classes</t>
   </si>
   <si>
-    <t>LIBORMonteCarloSimulationFromLIBORModel(final LIBORModel model, final MonteCarloProcess process)</t>
-  </si>
-  <si>
-    <t>deprecated</t>
-  </si>
-  <si>
-    <t>Refactorings of Methods (e.g. method signature or method name).</t>
-  </si>
-  <si>
-    <t>size of randomVariables int to long (will be considred later)</t>
-  </si>
-  <si>
-    <t>For 1D random number generators.</t>
+    <t>LIBORMonteCarloSimulationFromLIBORModel - constructor depreacted</t>
+  </si>
+  <si>
+    <t>TermStructureFactorLoadingsModelInterface</t>
+  </si>
+  <si>
+    <t>TermStructureFactorLoadingsModel</t>
+  </si>
+  <si>
+    <t>TermStructureFactorLoadingsModelParametricnterface</t>
+  </si>
+  <si>
+    <t>TermStructureFactorLoadingsModelParametric</t>
+  </si>
+  <si>
+    <t>TermStructureCovarianceModelInterface</t>
+  </si>
+  <si>
+    <t>TermStructureCovarianceModel</t>
+  </si>
+  <si>
+    <t>TermStructureTenorTimeScalingInterface</t>
+  </si>
+  <si>
+    <t>TermStructureTenorTimeScaling</t>
+  </si>
+  <si>
+    <t>net.finmath.montecarlo.interestrate.models.covariance</t>
+  </si>
+  <si>
+    <t>finmath-lib refactoring 4.x to 5.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -275,6 +296,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -317,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -329,9 +358,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -347,7 +377,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -643,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA599C8B-EB72-AF45-A360-A73F96FC6FB1}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,12 +687,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>40</v>
@@ -677,18 +707,15 @@
       <c r="A8" t="s">
         <v>38</v>
       </c>
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>59</v>
+    <row r="12" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -698,10 +725,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A833A924-41AF-4F4B-B135-14135420801F}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -761,19 +788,66 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
+      <c r="B8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
-      <c r="E9" s="9"/>
+      <c r="B9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
+      <c r="B10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E11" s="9"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="F11" s="9"/>
     </row>
     <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -784,27 +858,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
-      <c r="E15" s="9"/>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
       <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -813,19 +879,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11CCC08-C165-A14C-8682-5C60C2FEEEEC}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="93.5" customWidth="1"/>
-    <col min="5" max="5" width="63.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="63.33203125" customWidth="1"/>
     <col min="6" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="33.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.83203125" bestFit="1" customWidth="1"/>
@@ -833,7 +898,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="10" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -905,69 +970,66 @@
         <v>21</v>
       </c>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" t="s">
-        <v>53</v>
-      </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+        <v>48</v>
+      </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D28" t="s">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
         <v>56</v>
-      </c>
-      <c r="E28" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>